<commit_message>
Edited the code and added 3new classes in the script package
</commit_message>
<xml_diff>
--- a/src/main/resources/emsigner-credentials.xlsx
+++ b/src/main/resources/emsigner-credentials.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2775" windowWidth="14835" windowHeight="6495"/>
+    <workbookView windowHeight="6495" windowWidth="14835" xWindow="0" yWindow="2775"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginErrCheck" sheetId="28" r:id="rId1"/>
-    <sheet name="Credentials" sheetId="4" r:id="rId2"/>
-    <sheet name="Encrypt" sheetId="6" r:id="rId3"/>
-    <sheet name="Decrypt" sheetId="7" r:id="rId4"/>
-    <sheet name="Form16" sheetId="12" r:id="rId5"/>
-    <sheet name="Form" sheetId="14" r:id="rId6"/>
-    <sheet name="Dashboard" sheetId="15" r:id="rId7"/>
-    <sheet name="AnyDoc" sheetId="17" r:id="rId8"/>
-    <sheet name="BulkDoc" sheetId="20" r:id="rId9"/>
-    <sheet name="AdminSettings" sheetId="22" r:id="rId10"/>
-    <sheet name="Settings" sheetId="23" r:id="rId11"/>
-    <sheet name="PlanPricing" sheetId="24" r:id="rId12"/>
-    <sheet name="WFExternalFile" sheetId="26" r:id="rId13"/>
+    <sheet name="LoginErrCheck" r:id="rId1" sheetId="28"/>
+    <sheet name="Credentials" r:id="rId2" sheetId="4"/>
+    <sheet name="Encrypt" r:id="rId3" sheetId="6"/>
+    <sheet name="Decrypt" r:id="rId4" sheetId="7"/>
+    <sheet name="Form16" r:id="rId5" sheetId="12"/>
+    <sheet name="Form" r:id="rId6" sheetId="14"/>
+    <sheet name="Dashboard" r:id="rId7" sheetId="15"/>
+    <sheet name="AnyDoc" r:id="rId8" sheetId="17"/>
+    <sheet name="BulkDoc" r:id="rId9" sheetId="20"/>
+    <sheet name="AdminSettings" r:id="rId10" sheetId="22"/>
+    <sheet name="Settings" r:id="rId11" sheetId="23"/>
+    <sheet name="PlanPricing" r:id="rId12" sheetId="24"/>
+    <sheet name="WFExternalFile" r:id="rId13" sheetId="26"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="208">
   <si>
     <t>TC_ID</t>
   </si>
@@ -657,6 +657,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -721,30 +722,30 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -758,10 +759,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -919,7 +920,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -928,13 +929,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -944,7 +945,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -953,7 +954,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -962,7 +963,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -972,12 +973,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1008,7 +1009,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1027,7 +1028,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1039,8 +1040,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
@@ -1048,9 +1049,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1185,18 +1186,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="testem048@gmail.com"/>
-    <hyperlink ref="E3" r:id="rId2" display="testem048@gmail.com"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink display="testem048@gmail.com" r:id="rId1" ref="E2"/>
+    <hyperlink display="testem048@gmail.com" r:id="rId2" ref="E3"/>
+    <hyperlink r:id="rId3" ref="E5"/>
+    <hyperlink r:id="rId4" ref="E4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
@@ -1204,9 +1205,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="53.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1648,14 +1649,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H9"/>
@@ -1663,10 +1664,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="45.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1905,15 +1906,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H2"/>
@@ -1921,10 +1922,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2083,15 +2084,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="O2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
@@ -2099,8 +2100,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="47.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2202,13 +2203,13 @@
       <c r="H4" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
@@ -2216,8 +2217,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2296,16 +2297,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="E3"/>
+    <hyperlink r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -2313,9 +2314,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="47.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="47.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2606,16 +2607,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G7" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId2" ref="G7"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -2623,9 +2624,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="47.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="47.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2836,16 +2837,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G6" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId2" ref="G6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H9"/>
@@ -2853,10 +2854,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="61.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="61.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3095,15 +3096,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="E7"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
@@ -3111,9 +3112,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="61.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="61.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3191,13 +3192,13 @@
       <c r="H3" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -3232,13 +3233,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H5"/>
@@ -3272,7 +3273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -3377,13 +3378,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H7"/>
@@ -3391,9 +3392,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="61.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="61.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3580,8 +3581,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="E7"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>